<commit_message>
update test cases for LPH_V1.9.0 smoke/sanity test run.
</commit_message>
<xml_diff>
--- a/SystemTest/SmokeSanityExecutionResultV1.48.9.xlsx
+++ b/SystemTest/SmokeSanityExecutionResultV1.48.9.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\QA\AutomationTest\SystemTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationGIT\SystemTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="6480" windowHeight="7905"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="6480" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -174,8 +174,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,8 +199,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -216,6 +224,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -247,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -256,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +562,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +574,7 @@
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,13 +598,13 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="3">
@@ -594,13 +617,13 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3">
@@ -613,13 +636,13 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="3">
@@ -634,13 +657,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="3">
@@ -652,18 +675,18 @@
       <c r="F5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="3">
@@ -678,13 +701,13 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="3">
@@ -697,13 +720,13 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="3">
@@ -715,7 +738,7 @@
       <c r="F8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J8" t="s">
@@ -723,13 +746,13 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="3">
@@ -744,13 +767,13 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="3">
@@ -765,13 +788,13 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="3">
@@ -784,13 +807,13 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="3">
@@ -803,13 +826,13 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="3">
@@ -824,13 +847,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="3">
@@ -845,13 +868,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="3">
@@ -866,13 +889,13 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="8" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="3">
@@ -887,13 +910,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="8" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D17" s="3">
@@ -906,13 +929,13 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="8" t="s">
         <v>46</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D18" s="3">
@@ -927,13 +950,13 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="3">
@@ -949,6 +972,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>